<commit_message>
Ejemplos, inicio de aplicacion
</commit_message>
<xml_diff>
--- a/datos/billetes_monedas_publico.xlsx
+++ b/datos/billetes_monedas_publico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanpablolopezescamilla/Documents/Tesis/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDFE906-9C7D-454F-891E-A96256F56152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DAF985-F88F-B348-B0CF-794EC2EA8F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Banco de México</t>
   </si>
   <si>
-    <t>Agregados monetarios y activos financieros internos</t>
-  </si>
-  <si>
-    <t>Agregados monetarios (metodología 2018)</t>
-  </si>
-  <si>
-    <t>Fecha de consulta: 20/08/2022 09:00:56</t>
+    <t>Fecha de consulta: 19/02/2023 05:48:21</t>
   </si>
   <si>
     <t>Título</t>
@@ -43,7 +37,7 @@
     <t>Periodo disponible</t>
   </si>
   <si>
-    <t>Dic 2000 - Jun 2022</t>
+    <t>Dic 2000 - Dic 2022</t>
   </si>
   <si>
     <t>Periodicidad</t>
@@ -71,9 +65,6 @@
   </si>
   <si>
     <t>Tipo de información</t>
-  </si>
-  <si>
-    <t>Niveles</t>
   </si>
   <si>
     <t>Fecha</t>
@@ -170,7 +161,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -195,6 +185,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B277"/>
+  <dimension ref="A1:B311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -526,2160 +517,2280 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
-    </row>
-    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="7"/>
-    </row>
-    <row r="17" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="B18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>36861</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>182002892.25999999</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>36892</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>164450655.59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>36923</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>159626906.97</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="11">
+      <c r="A22" s="10">
         <v>36951</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>160268715.53999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="11">
+      <c r="A23" s="10">
         <v>36982</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <v>157791528.71000001</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="11">
+      <c r="A24" s="10">
         <v>37012</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <v>160310092.46000001</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="11">
+      <c r="A25" s="10">
         <v>37043</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>163257579.13999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="11">
+      <c r="A26" s="10">
         <v>37073</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="9">
         <v>161993494.49000001</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="11">
+      <c r="A27" s="10">
         <v>37104</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="9">
         <v>162163788.55000001</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="11">
+      <c r="A28" s="10">
         <v>37135</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <v>164899050.86000001</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="11">
+      <c r="A29" s="10">
         <v>37165</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="9">
         <v>163829180.36000001</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="11">
+      <c r="A30" s="10">
         <v>37196</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>173831135.97999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="11">
+      <c r="A31" s="10">
         <v>37226</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <v>198880321.83000001</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="11">
+      <c r="A32" s="10">
         <v>37257</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="9">
         <v>186542107.47</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="11">
+      <c r="A33" s="10">
         <v>37288</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="9">
         <v>181646178.02000001</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="11">
+      <c r="A34" s="10">
         <v>37316</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="9">
         <v>190998569.96000001</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="11">
+      <c r="A35" s="10">
         <v>37347</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="9">
         <v>182583041.88999999</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="11">
+      <c r="A36" s="10">
         <v>37377</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="9">
         <v>190993341</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="11">
+      <c r="A37" s="10">
         <v>37408</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="9">
         <v>191930698.49000001</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="11">
+      <c r="A38" s="10">
         <v>37438</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="9">
         <v>189743385.41</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="11">
+      <c r="A39" s="10">
         <v>37469</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="9">
         <v>190385779.81</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="11">
+      <c r="A40" s="10">
         <v>37500</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="9">
         <v>192004597.69</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="11">
+      <c r="A41" s="10">
         <v>37530</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="9">
         <v>191783884.00999999</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="11">
+      <c r="A42" s="10">
         <v>37561</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="9">
         <v>202232498.28999999</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="11">
+      <c r="A43" s="10">
         <v>37591</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="9">
         <v>232188483.5</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="11">
+      <c r="A44" s="10">
         <v>37622</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="9">
         <v>223470450.94999999</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="11">
+      <c r="A45" s="10">
         <v>37653</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="9">
         <v>218346630.12</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="11">
+      <c r="A46" s="10">
         <v>37681</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="9">
         <v>213648958.12</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="11">
+      <c r="A47" s="10">
         <v>37712</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="9">
         <v>213752231.80000001</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="11">
+      <c r="A48" s="10">
         <v>37742</v>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="9">
         <v>218761401.93000001</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="11">
+      <c r="A49" s="10">
         <v>37773</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <v>216884802.19999999</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="11">
+      <c r="A50" s="10">
         <v>37803</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="9">
         <v>214789289.84999999</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="11">
+      <c r="A51" s="10">
         <v>37834</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="9">
         <v>216930860.72999999</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="11">
+      <c r="A52" s="10">
         <v>37865</v>
       </c>
-      <c r="B52" s="10">
+      <c r="B52" s="9">
         <v>214324892.91999999</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="11">
+      <c r="A53" s="10">
         <v>37895</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="9">
         <v>221869029.12</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="11">
+      <c r="A54" s="10">
         <v>37926</v>
       </c>
-      <c r="B54" s="10">
+      <c r="B54" s="9">
         <v>228963361.41999999</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="11">
+      <c r="A55" s="10">
         <v>37956</v>
       </c>
-      <c r="B55" s="10">
+      <c r="B55" s="9">
         <v>263547762.19</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="11">
+      <c r="A56" s="10">
         <v>37987</v>
       </c>
-      <c r="B56" s="10">
+      <c r="B56" s="9">
         <v>251684813.00999999</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="11">
+      <c r="A57" s="10">
         <v>38018</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B57" s="9">
         <v>246658268.21000001</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="11">
+      <c r="A58" s="10">
         <v>38047</v>
       </c>
-      <c r="B58" s="10">
+      <c r="B58" s="9">
         <v>239594162.05000001</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="11">
+      <c r="A59" s="10">
         <v>38078</v>
       </c>
-      <c r="B59" s="10">
+      <c r="B59" s="9">
         <v>247552468.91</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="11">
+      <c r="A60" s="10">
         <v>38108</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B60" s="9">
         <v>250478083.71000001</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="11">
+      <c r="A61" s="10">
         <v>38139</v>
       </c>
-      <c r="B61" s="10">
+      <c r="B61" s="9">
         <v>249958690.83000001</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="11">
+      <c r="A62" s="10">
         <v>38169</v>
       </c>
-      <c r="B62" s="10">
+      <c r="B62" s="9">
         <v>253209836.94999999</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="11">
+      <c r="A63" s="10">
         <v>38200</v>
       </c>
-      <c r="B63" s="10">
+      <c r="B63" s="9">
         <v>247265497.36000001</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="11">
+      <c r="A64" s="10">
         <v>38231</v>
       </c>
-      <c r="B64" s="10">
+      <c r="B64" s="9">
         <v>247083323.91</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="11">
+      <c r="A65" s="10">
         <v>38261</v>
       </c>
-      <c r="B65" s="10">
+      <c r="B65" s="9">
         <v>256441531.88</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="11">
+      <c r="A66" s="10">
         <v>38292</v>
       </c>
-      <c r="B66" s="10">
+      <c r="B66" s="9">
         <v>261408307.13</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="11">
+      <c r="A67" s="10">
         <v>38322</v>
       </c>
-      <c r="B67" s="10">
+      <c r="B67" s="9">
         <v>301114461.24000001</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="11">
+      <c r="A68" s="10">
         <v>38353</v>
       </c>
-      <c r="B68" s="10">
+      <c r="B68" s="9">
         <v>286242842.88999999</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="11">
+      <c r="A69" s="10">
         <v>38384</v>
       </c>
-      <c r="B69" s="10">
+      <c r="B69" s="9">
         <v>279475469.58999997</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="11">
+      <c r="A70" s="10">
         <v>38412</v>
       </c>
-      <c r="B70" s="10">
+      <c r="B70" s="9">
         <v>275748786.43000001</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="11">
+      <c r="A71" s="10">
         <v>38443</v>
       </c>
-      <c r="B71" s="10">
+      <c r="B71" s="9">
         <v>276874469.88</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="11">
+      <c r="A72" s="10">
         <v>38473</v>
       </c>
-      <c r="B72" s="10">
+      <c r="B72" s="9">
         <v>278015061.16000003</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="11">
+      <c r="A73" s="10">
         <v>38504</v>
       </c>
-      <c r="B73" s="10">
+      <c r="B73" s="9">
         <v>280410187.80000001</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="11">
+      <c r="A74" s="10">
         <v>38534</v>
       </c>
-      <c r="B74" s="10">
+      <c r="B74" s="9">
         <v>283271832.68000001</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="11">
+      <c r="A75" s="10">
         <v>38565</v>
       </c>
-      <c r="B75" s="10">
+      <c r="B75" s="9">
         <v>274719290.68000001</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="11">
+      <c r="A76" s="10">
         <v>38596</v>
       </c>
-      <c r="B76" s="10">
+      <c r="B76" s="9">
         <v>282318750.19</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="11">
+      <c r="A77" s="10">
         <v>38626</v>
       </c>
-      <c r="B77" s="10">
+      <c r="B77" s="9">
         <v>285511997</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="11">
+      <c r="A78" s="10">
         <v>38657</v>
       </c>
-      <c r="B78" s="10">
+      <c r="B78" s="9">
         <v>290355447.31</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="11">
+      <c r="A79" s="10">
         <v>38687</v>
       </c>
-      <c r="B79" s="10">
+      <c r="B79" s="9">
         <v>336073254.26999998</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="11">
+      <c r="A80" s="10">
         <v>38718</v>
       </c>
-      <c r="B80" s="10">
+      <c r="B80" s="9">
         <v>318653696.08999997</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="11">
+      <c r="A81" s="10">
         <v>38749</v>
       </c>
-      <c r="B81" s="10">
+      <c r="B81" s="9">
         <v>312792724.95999998</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="11">
+      <c r="A82" s="10">
         <v>38777</v>
       </c>
-      <c r="B82" s="10">
+      <c r="B82" s="9">
         <v>318642680.95999998</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="11">
+      <c r="A83" s="10">
         <v>38808</v>
       </c>
-      <c r="B83" s="10">
+      <c r="B83" s="9">
         <v>318855199.41000003</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="11">
+      <c r="A84" s="10">
         <v>38838</v>
       </c>
-      <c r="B84" s="10">
+      <c r="B84" s="9">
         <v>322666481.69999999</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="11">
+      <c r="A85" s="10">
         <v>38869</v>
       </c>
-      <c r="B85" s="10">
+      <c r="B85" s="9">
         <v>332355752.86000001</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="11">
+      <c r="A86" s="10">
         <v>38899</v>
       </c>
-      <c r="B86" s="10">
+      <c r="B86" s="9">
         <v>332296189.49000001</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="11">
+      <c r="A87" s="10">
         <v>38930</v>
       </c>
-      <c r="B87" s="10">
+      <c r="B87" s="9">
         <v>323269985.51999998</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="11">
+      <c r="A88" s="10">
         <v>38961</v>
       </c>
-      <c r="B88" s="10">
+      <c r="B88" s="9">
         <v>329907360.81</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="11">
+      <c r="A89" s="10">
         <v>38991</v>
       </c>
-      <c r="B89" s="10">
+      <c r="B89" s="9">
         <v>327995456.67000002</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="11">
+      <c r="A90" s="10">
         <v>39022</v>
       </c>
-      <c r="B90" s="10">
+      <c r="B90" s="9">
         <v>347357948.69</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="11">
+      <c r="A91" s="10">
         <v>39052</v>
       </c>
-      <c r="B91" s="10">
+      <c r="B91" s="9">
         <v>389471396.20999998</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="11">
+      <c r="A92" s="10">
         <v>39083</v>
       </c>
-      <c r="B92" s="10">
+      <c r="B92" s="9">
         <v>366744139.45999998</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="11">
+      <c r="A93" s="10">
         <v>39114</v>
       </c>
-      <c r="B93" s="10">
+      <c r="B93" s="9">
         <v>359358746.98000002</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="11">
+      <c r="A94" s="10">
         <v>39142</v>
       </c>
-      <c r="B94" s="10">
+      <c r="B94" s="9">
         <v>367282511.55000001</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="11">
+      <c r="A95" s="10">
         <v>39173</v>
       </c>
-      <c r="B95" s="10">
+      <c r="B95" s="9">
         <v>359960622</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="11">
+      <c r="A96" s="10">
         <v>39203</v>
       </c>
-      <c r="B96" s="10">
+      <c r="B96" s="9">
         <v>359993937.27999997</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="11">
+      <c r="A97" s="10">
         <v>39234</v>
       </c>
-      <c r="B97" s="10">
+      <c r="B97" s="9">
         <v>366151931.67000002</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="11">
+      <c r="A98" s="10">
         <v>39264</v>
       </c>
-      <c r="B98" s="10">
+      <c r="B98" s="9">
         <v>366749095.31999999</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="11">
+      <c r="A99" s="10">
         <v>39295</v>
       </c>
-      <c r="B99" s="10">
+      <c r="B99" s="9">
         <v>367954618.20999998</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="11">
+      <c r="A100" s="10">
         <v>39326</v>
       </c>
-      <c r="B100" s="10">
+      <c r="B100" s="9">
         <v>367299957.20999998</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="11">
+      <c r="A101" s="10">
         <v>39356</v>
       </c>
-      <c r="B101" s="10">
+      <c r="B101" s="9">
         <v>364920297.38</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="11">
+      <c r="A102" s="10">
         <v>39387</v>
       </c>
-      <c r="B102" s="10">
+      <c r="B102" s="9">
         <v>382319560.48000002</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="11">
+      <c r="A103" s="10">
         <v>39417</v>
       </c>
-      <c r="B103" s="10">
+      <c r="B103" s="9">
         <v>429979589.86000001</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="11">
+      <c r="A104" s="10">
         <v>39448</v>
       </c>
-      <c r="B104" s="10">
+      <c r="B104" s="9">
         <v>405979634.18000001</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="11">
+      <c r="A105" s="10">
         <v>39479</v>
       </c>
-      <c r="B105" s="10">
+      <c r="B105" s="9">
         <v>403392949.37</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="11">
+      <c r="A106" s="10">
         <v>39508</v>
       </c>
-      <c r="B106" s="10">
+      <c r="B106" s="9">
         <v>397941337.44</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="11">
+      <c r="A107" s="10">
         <v>39539</v>
       </c>
-      <c r="B107" s="10">
+      <c r="B107" s="9">
         <v>393084215.18000001</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="11">
+      <c r="A108" s="10">
         <v>39569</v>
       </c>
-      <c r="B108" s="10">
+      <c r="B108" s="9">
         <v>399608152.98000002</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="11">
+      <c r="A109" s="10">
         <v>39600</v>
       </c>
-      <c r="B109" s="10">
+      <c r="B109" s="9">
         <v>395448496.39999998</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="11">
+      <c r="A110" s="10">
         <v>39630</v>
       </c>
-      <c r="B110" s="10">
+      <c r="B110" s="9">
         <v>403494699.43000001</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="11">
+      <c r="A111" s="10">
         <v>39661</v>
       </c>
-      <c r="B111" s="10">
+      <c r="B111" s="9">
         <v>404437961.64999998</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="11">
+      <c r="A112" s="10">
         <v>39692</v>
       </c>
-      <c r="B112" s="10">
+      <c r="B112" s="9">
         <v>403569205.77999997</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="11">
+      <c r="A113" s="10">
         <v>39722</v>
       </c>
-      <c r="B113" s="10">
+      <c r="B113" s="9">
         <v>423880790.67000002</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="11">
+      <c r="A114" s="10">
         <v>39753</v>
       </c>
-      <c r="B114" s="10">
+      <c r="B114" s="9">
         <v>436038650.30000001</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="11">
+      <c r="A115" s="10">
         <v>39783</v>
       </c>
-      <c r="B115" s="10">
+      <c r="B115" s="9">
         <v>494352262.83999997</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="11">
+      <c r="A116" s="10">
         <v>39814</v>
       </c>
-      <c r="B116" s="10">
+      <c r="B116" s="9">
         <v>479699526.61000001</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="11">
+      <c r="A117" s="10">
         <v>39845</v>
       </c>
-      <c r="B117" s="10">
+      <c r="B117" s="9">
         <v>475258808.31999999</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="11">
+      <c r="A118" s="10">
         <v>39873</v>
       </c>
-      <c r="B118" s="10">
+      <c r="B118" s="9">
         <v>471454247.69</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="11">
+      <c r="A119" s="10">
         <v>39904</v>
       </c>
-      <c r="B119" s="10">
+      <c r="B119" s="9">
         <v>470514879.19</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="11">
+      <c r="A120" s="10">
         <v>39934</v>
       </c>
-      <c r="B120" s="10">
+      <c r="B120" s="9">
         <v>473891910.75999999</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="11">
+      <c r="A121" s="10">
         <v>39965</v>
       </c>
-      <c r="B121" s="10">
+      <c r="B121" s="9">
         <v>468343824.42000002</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="11">
+      <c r="A122" s="10">
         <v>39995</v>
       </c>
-      <c r="B122" s="10">
+      <c r="B122" s="9">
         <v>474749818.24000001</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="11">
+      <c r="A123" s="10">
         <v>40026</v>
       </c>
-      <c r="B123" s="10">
+      <c r="B123" s="9">
         <v>464943903.94999999</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="11">
+      <c r="A124" s="10">
         <v>40057</v>
       </c>
-      <c r="B124" s="10">
+      <c r="B124" s="9">
         <v>460087018.01999998</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="11">
+      <c r="A125" s="10">
         <v>40087</v>
       </c>
-      <c r="B125" s="10">
+      <c r="B125" s="9">
         <v>468186286.58999997</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="11">
+      <c r="A126" s="10">
         <v>40118</v>
       </c>
-      <c r="B126" s="10">
+      <c r="B126" s="9">
         <v>478278462.31</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="11">
+      <c r="A127" s="10">
         <v>40148</v>
       </c>
-      <c r="B127" s="10">
+      <c r="B127" s="9">
         <v>536824462.48000002</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="11">
+      <c r="A128" s="10">
         <v>40179</v>
       </c>
-      <c r="B128" s="10">
+      <c r="B128" s="9">
         <v>519517391.08999997</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="11">
+      <c r="A129" s="10">
         <v>40210</v>
       </c>
-      <c r="B129" s="10">
+      <c r="B129" s="9">
         <v>513018657.31999999</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="11">
+      <c r="A130" s="10">
         <v>40238</v>
       </c>
-      <c r="B130" s="10">
+      <c r="B130" s="9">
         <v>516527701.36000001</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="11">
+      <c r="A131" s="10">
         <v>40269</v>
       </c>
-      <c r="B131" s="10">
+      <c r="B131" s="9">
         <v>508527032.25999999</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="11">
+      <c r="A132" s="10">
         <v>40299</v>
       </c>
-      <c r="B132" s="10">
+      <c r="B132" s="9">
         <v>517335155.51999998</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="11">
+      <c r="A133" s="10">
         <v>40330</v>
       </c>
-      <c r="B133" s="10">
+      <c r="B133" s="9">
         <v>514675633.80000001</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="11">
+      <c r="A134" s="10">
         <v>40360</v>
       </c>
-      <c r="B134" s="10">
+      <c r="B134" s="9">
         <v>525939253.52999997</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="11">
+      <c r="A135" s="10">
         <v>40391</v>
       </c>
-      <c r="B135" s="10">
+      <c r="B135" s="9">
         <v>518748981.11000001</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="11">
+      <c r="A136" s="10">
         <v>40422</v>
       </c>
-      <c r="B136" s="10">
+      <c r="B136" s="9">
         <v>514012112.31</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="11">
+      <c r="A137" s="10">
         <v>40452</v>
       </c>
-      <c r="B137" s="10">
+      <c r="B137" s="9">
         <v>522847754.47000003</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="11">
+      <c r="A138" s="10">
         <v>40483</v>
       </c>
-      <c r="B138" s="10">
+      <c r="B138" s="9">
         <v>531623121.05000001</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="11">
+      <c r="A139" s="10">
         <v>40513</v>
       </c>
-      <c r="B139" s="10">
+      <c r="B139" s="9">
         <v>599058360.71000004</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="11">
+      <c r="A140" s="10">
         <v>40544</v>
       </c>
-      <c r="B140" s="10">
+      <c r="B140" s="9">
         <v>575338818.82000005</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="11">
+      <c r="A141" s="10">
         <v>40575</v>
       </c>
-      <c r="B141" s="10">
+      <c r="B141" s="9">
         <v>568762276.10000002</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="11">
+      <c r="A142" s="10">
         <v>40603</v>
       </c>
-      <c r="B142" s="10">
+      <c r="B142" s="9">
         <v>559812846.80999994</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="11">
+      <c r="A143" s="10">
         <v>40634</v>
       </c>
-      <c r="B143" s="10">
+      <c r="B143" s="9">
         <v>563870244.16999996</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="11">
+      <c r="A144" s="10">
         <v>40664</v>
       </c>
-      <c r="B144" s="10">
+      <c r="B144" s="9">
         <v>563755300.34000003</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="11">
+      <c r="A145" s="10">
         <v>40695</v>
       </c>
-      <c r="B145" s="10">
+      <c r="B145" s="9">
         <v>561297800.01999998</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="11">
+      <c r="A146" s="10">
         <v>40725</v>
       </c>
-      <c r="B146" s="10">
+      <c r="B146" s="9">
         <v>568155834.26999998</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="11">
+      <c r="A147" s="10">
         <v>40756</v>
       </c>
-      <c r="B147" s="10">
+      <c r="B147" s="9">
         <v>561100355.01999998</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="11">
+      <c r="A148" s="10">
         <v>40787</v>
       </c>
-      <c r="B148" s="10">
+      <c r="B148" s="9">
         <v>568616362.51999998</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="11">
+      <c r="A149" s="10">
         <v>40817</v>
       </c>
-      <c r="B149" s="10">
+      <c r="B149" s="9">
         <v>575634865.69000006</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="11">
+      <c r="A150" s="10">
         <v>40848</v>
       </c>
-      <c r="B150" s="10">
+      <c r="B150" s="9">
         <v>588599492.91999996</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="11">
+      <c r="A151" s="10">
         <v>40878</v>
       </c>
-      <c r="B151" s="10">
+      <c r="B151" s="9">
         <v>665525155.73000002</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="11">
+      <c r="A152" s="10">
         <v>40909</v>
       </c>
-      <c r="B152" s="10">
+      <c r="B152" s="9">
         <v>639251863.13</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="11">
+      <c r="A153" s="10">
         <v>40940</v>
       </c>
-      <c r="B153" s="10">
+      <c r="B153" s="9">
         <v>634676648.19000006</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="11">
+      <c r="A154" s="10">
         <v>40969</v>
       </c>
-      <c r="B154" s="10">
+      <c r="B154" s="9">
         <v>642798261.52999997</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="11">
+      <c r="A155" s="10">
         <v>41000</v>
       </c>
-      <c r="B155" s="10">
+      <c r="B155" s="9">
         <v>646470935.59000003</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="11">
+      <c r="A156" s="10">
         <v>41030</v>
       </c>
-      <c r="B156" s="10">
+      <c r="B156" s="9">
         <v>656623534.70000005</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="11">
+      <c r="A157" s="10">
         <v>41061</v>
       </c>
-      <c r="B157" s="10">
+      <c r="B157" s="9">
         <v>669519731.92999995</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="11">
+      <c r="A158" s="10">
         <v>41091</v>
       </c>
-      <c r="B158" s="10">
+      <c r="B158" s="9">
         <v>660889320.97000003</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="11">
+      <c r="A159" s="10">
         <v>41122</v>
       </c>
-      <c r="B159" s="10">
+      <c r="B159" s="9">
         <v>658074453.19000006</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="11">
+      <c r="A160" s="10">
         <v>41153</v>
       </c>
-      <c r="B160" s="10">
+      <c r="B160" s="9">
         <v>647570543.40999997</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="11">
+      <c r="A161" s="10">
         <v>41183</v>
       </c>
-      <c r="B161" s="10">
+      <c r="B161" s="9">
         <v>649644763.21000004</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" s="11">
+      <c r="A162" s="10">
         <v>41214</v>
       </c>
-      <c r="B162" s="10">
+      <c r="B162" s="9">
         <v>669497674.79999995</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="11">
+      <c r="A163" s="10">
         <v>41244</v>
       </c>
-      <c r="B163" s="10">
+      <c r="B163" s="9">
         <v>733451725.10000002</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" s="11">
+      <c r="A164" s="10">
         <v>41275</v>
       </c>
-      <c r="B164" s="10">
+      <c r="B164" s="9">
         <v>695950944.64999998</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" s="11">
+      <c r="A165" s="10">
         <v>41306</v>
       </c>
-      <c r="B165" s="10">
+      <c r="B165" s="9">
         <v>686550500.71000004</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="11">
+      <c r="A166" s="10">
         <v>41334</v>
       </c>
-      <c r="B166" s="10">
+      <c r="B166" s="9">
         <v>691564113.60000002</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="11">
+      <c r="A167" s="10">
         <v>41365</v>
       </c>
-      <c r="B167" s="10">
+      <c r="B167" s="9">
         <v>678914429.32000005</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="11">
+      <c r="A168" s="10">
         <v>41395</v>
       </c>
-      <c r="B168" s="10">
+      <c r="B168" s="9">
         <v>688578205.17999995</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" s="11">
+      <c r="A169" s="10">
         <v>41426</v>
       </c>
-      <c r="B169" s="10">
+      <c r="B169" s="9">
         <v>686576437.00999999</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" s="11">
+      <c r="A170" s="10">
         <v>41456</v>
       </c>
-      <c r="B170" s="10">
+      <c r="B170" s="9">
         <v>680113672.70000005</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" s="11">
+      <c r="A171" s="10">
         <v>41487</v>
       </c>
-      <c r="B171" s="10">
+      <c r="B171" s="9">
         <v>683323703.26999998</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="11">
+      <c r="A172" s="10">
         <v>41518</v>
       </c>
-      <c r="B172" s="10">
+      <c r="B172" s="9">
         <v>681670380.29999995</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" s="11">
+      <c r="A173" s="10">
         <v>41548</v>
       </c>
-      <c r="B173" s="10">
+      <c r="B173" s="9">
         <v>687989636.30999994</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" s="11">
+      <c r="A174" s="10">
         <v>41579</v>
       </c>
-      <c r="B174" s="10">
+      <c r="B174" s="9">
         <v>711274007.78999996</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="11">
+      <c r="A175" s="10">
         <v>41609</v>
       </c>
-      <c r="B175" s="10">
+      <c r="B175" s="9">
         <v>792262602.26999998</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="11">
+      <c r="A176" s="10">
         <v>41640</v>
       </c>
-      <c r="B176" s="10">
+      <c r="B176" s="9">
         <v>769604674.63999999</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="11">
+      <c r="A177" s="10">
         <v>41671</v>
       </c>
-      <c r="B177" s="10">
+      <c r="B177" s="9">
         <v>771791358.49000001</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="11">
+      <c r="A178" s="10">
         <v>41699</v>
       </c>
-      <c r="B178" s="10">
+      <c r="B178" s="9">
         <v>766960190.94000006</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="11">
+      <c r="A179" s="10">
         <v>41730</v>
       </c>
-      <c r="B179" s="10">
+      <c r="B179" s="9">
         <v>768733613.5</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="11">
+      <c r="A180" s="10">
         <v>41760</v>
       </c>
-      <c r="B180" s="10">
+      <c r="B180" s="9">
         <v>777256249.94000006</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" s="11">
+      <c r="A181" s="10">
         <v>41791</v>
       </c>
-      <c r="B181" s="10">
+      <c r="B181" s="9">
         <v>783001969.27999997</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="11">
+      <c r="A182" s="10">
         <v>41821</v>
       </c>
-      <c r="B182" s="10">
+      <c r="B182" s="9">
         <v>783208664.63999999</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" s="11">
+      <c r="A183" s="10">
         <v>41852</v>
       </c>
-      <c r="B183" s="10">
+      <c r="B183" s="9">
         <v>787820209.95000005</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" s="11">
+      <c r="A184" s="10">
         <v>41883</v>
       </c>
-      <c r="B184" s="10">
+      <c r="B184" s="9">
         <v>788660080.96000004</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" s="11">
+      <c r="A185" s="10">
         <v>41913</v>
       </c>
-      <c r="B185" s="10">
+      <c r="B185" s="9">
         <v>811715734.65999997</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" s="11">
+      <c r="A186" s="10">
         <v>41944</v>
       </c>
-      <c r="B186" s="10">
+      <c r="B186" s="9">
         <v>829468731.91999996</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" s="11">
+      <c r="A187" s="10">
         <v>41974</v>
       </c>
-      <c r="B187" s="10">
+      <c r="B187" s="9">
         <v>928051802.60000002</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="11">
+      <c r="A188" s="10">
         <v>42005</v>
       </c>
-      <c r="B188" s="10">
+      <c r="B188" s="9">
         <v>910089542.75</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" s="11">
+      <c r="A189" s="10">
         <v>42036</v>
       </c>
-      <c r="B189" s="10">
+      <c r="B189" s="9">
         <v>917404455.47000003</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="11">
+      <c r="A190" s="10">
         <v>42064</v>
       </c>
-      <c r="B190" s="10">
+      <c r="B190" s="9">
         <v>931897661.15999997</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" s="11">
+      <c r="A191" s="10">
         <v>42095</v>
       </c>
-      <c r="B191" s="10">
+      <c r="B191" s="9">
         <v>933091994.55999994</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" s="11">
+      <c r="A192" s="10">
         <v>42125</v>
       </c>
-      <c r="B192" s="10">
+      <c r="B192" s="9">
         <v>943056323.87</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" s="11">
+      <c r="A193" s="10">
         <v>42156</v>
       </c>
-      <c r="B193" s="10">
+      <c r="B193" s="9">
         <v>946647963.63999999</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="11">
+      <c r="A194" s="10">
         <v>42186</v>
       </c>
-      <c r="B194" s="10">
+      <c r="B194" s="9">
         <v>961274296.79999995</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" s="11">
+      <c r="A195" s="10">
         <v>42217</v>
       </c>
-      <c r="B195" s="10">
+      <c r="B195" s="9">
         <v>964823694.95000005</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" s="11">
+      <c r="A196" s="10">
         <v>42248</v>
       </c>
-      <c r="B196" s="10">
+      <c r="B196" s="9">
         <v>956954871.90999997</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="11">
+      <c r="A197" s="10">
         <v>42278</v>
       </c>
-      <c r="B197" s="10">
+      <c r="B197" s="9">
         <v>975422285.13999999</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" s="11">
+      <c r="A198" s="10">
         <v>42309</v>
       </c>
-      <c r="B198" s="10">
+      <c r="B198" s="9">
         <v>993973732.41999996</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="11">
+      <c r="A199" s="10">
         <v>42339</v>
       </c>
-      <c r="B199" s="10">
+      <c r="B199" s="9">
         <v>1087271129.0999999</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" s="11">
+      <c r="A200" s="10">
         <v>42370</v>
       </c>
-      <c r="B200" s="10">
+      <c r="B200" s="9">
         <v>1067781583.92</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" s="11">
+      <c r="A201" s="10">
         <v>42401</v>
       </c>
-      <c r="B201" s="10">
+      <c r="B201" s="9">
         <v>1071562313.84</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" s="11">
+      <c r="A202" s="10">
         <v>42430</v>
       </c>
-      <c r="B202" s="10">
+      <c r="B202" s="9">
         <v>1064980086.67</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A203" s="11">
+      <c r="A203" s="10">
         <v>42461</v>
       </c>
-      <c r="B203" s="10">
+      <c r="B203" s="9">
         <v>1078102012.03</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="11">
+      <c r="A204" s="10">
         <v>42491</v>
       </c>
-      <c r="B204" s="10">
+      <c r="B204" s="9">
         <v>1095923235.6099999</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A205" s="11">
+      <c r="A205" s="10">
         <v>42522</v>
       </c>
-      <c r="B205" s="10">
+      <c r="B205" s="9">
         <v>1105334085.3</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A206" s="11">
+      <c r="A206" s="10">
         <v>42552</v>
       </c>
-      <c r="B206" s="10">
+      <c r="B206" s="9">
         <v>1116603722.21</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A207" s="11">
+      <c r="A207" s="10">
         <v>42583</v>
       </c>
-      <c r="B207" s="10">
+      <c r="B207" s="9">
         <v>1111377366.3599999</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A208" s="11">
+      <c r="A208" s="10">
         <v>42614</v>
       </c>
-      <c r="B208" s="10">
+      <c r="B208" s="9">
         <v>1124689216.21</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" s="11">
+      <c r="A209" s="10">
         <v>42644</v>
       </c>
-      <c r="B209" s="10">
+      <c r="B209" s="9">
         <v>1135595320.3299999</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" s="11">
+      <c r="A210" s="10">
         <v>42675</v>
       </c>
-      <c r="B210" s="10">
+      <c r="B210" s="9">
         <v>1157805654.1600001</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A211" s="11">
+      <c r="A211" s="10">
         <v>42705</v>
       </c>
-      <c r="B211" s="10">
+      <c r="B211" s="9">
         <v>1261697098.1700001</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A212" s="11">
+      <c r="A212" s="10">
         <v>42736</v>
       </c>
-      <c r="B212" s="10">
+      <c r="B212" s="9">
         <v>1236669605.8</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A213" s="11">
+      <c r="A213" s="10">
         <v>42767</v>
       </c>
-      <c r="B213" s="10">
+      <c r="B213" s="9">
         <v>1234574732.7</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A214" s="11">
+      <c r="A214" s="10">
         <v>42795</v>
       </c>
-      <c r="B214" s="10">
+      <c r="B214" s="9">
         <v>1236434261.05</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A215" s="11">
+      <c r="A215" s="10">
         <v>42826</v>
       </c>
-      <c r="B215" s="10">
+      <c r="B215" s="9">
         <v>1235342032.52</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A216" s="11">
+      <c r="A216" s="10">
         <v>42856</v>
       </c>
-      <c r="B216" s="10">
+      <c r="B216" s="9">
         <v>1234585812.53</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A217" s="11">
+      <c r="A217" s="10">
         <v>42887</v>
       </c>
-      <c r="B217" s="10">
+      <c r="B217" s="9">
         <v>1240499937.97</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A218" s="11">
+      <c r="A218" s="10">
         <v>42917</v>
       </c>
-      <c r="B218" s="10">
+      <c r="B218" s="9">
         <v>1238358805.5599999</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A219" s="11">
+      <c r="A219" s="10">
         <v>42948</v>
       </c>
-      <c r="B219" s="10">
+      <c r="B219" s="9">
         <v>1223080022.8499999</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A220" s="11">
+      <c r="A220" s="10">
         <v>42979</v>
       </c>
-      <c r="B220" s="10">
+      <c r="B220" s="9">
         <v>1226669132.47</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A221" s="11">
+      <c r="A221" s="10">
         <v>43009</v>
       </c>
-      <c r="B221" s="10">
+      <c r="B221" s="9">
         <v>1240531999.3199999</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A222" s="11">
+      <c r="A222" s="10">
         <v>43040</v>
       </c>
-      <c r="B222" s="10">
+      <c r="B222" s="9">
         <v>1257536648.6500001</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A223" s="11">
+      <c r="A223" s="10">
         <v>43070</v>
       </c>
-      <c r="B223" s="10">
+      <c r="B223" s="9">
         <v>1372883843.5599999</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A224" s="11">
+      <c r="A224" s="10">
         <v>43101</v>
       </c>
-      <c r="B224" s="10">
+      <c r="B224" s="9">
         <v>1337103548.5999999</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A225" s="11">
+      <c r="A225" s="10">
         <v>43132</v>
       </c>
-      <c r="B225" s="10">
+      <c r="B225" s="9">
         <v>1334882602.6099999</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A226" s="11">
+      <c r="A226" s="10">
         <v>43160</v>
       </c>
-      <c r="B226" s="10">
+      <c r="B226" s="9">
         <v>1356624271.3099999</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A227" s="11">
+      <c r="A227" s="10">
         <v>43191</v>
       </c>
-      <c r="B227" s="10">
+      <c r="B227" s="9">
         <v>1353271169.3800001</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A228" s="11">
+      <c r="A228" s="10">
         <v>43221</v>
       </c>
-      <c r="B228" s="10">
+      <c r="B228" s="9">
         <v>1362367307.02</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" s="11">
+      <c r="A229" s="10">
         <v>43252</v>
       </c>
-      <c r="B229" s="10">
+      <c r="B229" s="9">
         <v>1393414137.24</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" s="11">
+      <c r="A230" s="10">
         <v>43282</v>
       </c>
-      <c r="B230" s="10">
+      <c r="B230" s="9">
         <v>1380780883.99</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A231" s="11">
+      <c r="A231" s="10">
         <v>43313</v>
       </c>
-      <c r="B231" s="10">
+      <c r="B231" s="9">
         <v>1380344334.8699999</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A232" s="11">
+      <c r="A232" s="10">
         <v>43344</v>
       </c>
-      <c r="B232" s="10">
+      <c r="B232" s="9">
         <v>1366830626.23</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A233" s="11">
+      <c r="A233" s="10">
         <v>43374</v>
       </c>
-      <c r="B233" s="10">
+      <c r="B233" s="9">
         <v>1373773785.3099999</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A234" s="11">
+      <c r="A234" s="10">
         <v>43405</v>
       </c>
-      <c r="B234" s="10">
+      <c r="B234" s="9">
         <v>1407445049.2</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A235" s="11">
+      <c r="A235" s="10">
         <v>43435</v>
       </c>
-      <c r="B235" s="10">
+      <c r="B235" s="9">
         <v>1494948943.1600001</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A236" s="11">
+      <c r="A236" s="10">
         <v>43466</v>
       </c>
-      <c r="B236" s="10">
+      <c r="B236" s="9">
         <v>1442658585.3399999</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A237" s="11">
+      <c r="A237" s="10">
         <v>43497</v>
       </c>
-      <c r="B237" s="10">
+      <c r="B237" s="9">
         <v>1424312650.46</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A238" s="11">
+      <c r="A238" s="10">
         <v>43525</v>
       </c>
-      <c r="B238" s="10">
+      <c r="B238" s="9">
         <v>1417029864.0699999</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A239" s="11">
+      <c r="A239" s="10">
         <v>43556</v>
       </c>
-      <c r="B239" s="10">
+      <c r="B239" s="9">
         <v>1409808963.76</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A240" s="11">
+      <c r="A240" s="10">
         <v>43586</v>
       </c>
-      <c r="B240" s="10">
+      <c r="B240" s="9">
         <v>1423278734.7</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A241" s="11">
+      <c r="A241" s="10">
         <v>43617</v>
       </c>
-      <c r="B241" s="10">
+      <c r="B241" s="9">
         <v>1420639324</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A242" s="11">
+      <c r="A242" s="10">
         <v>43647</v>
       </c>
-      <c r="B242" s="10">
+      <c r="B242" s="9">
         <v>1403852286.1400001</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A243" s="11">
+      <c r="A243" s="10">
         <v>43678</v>
       </c>
-      <c r="B243" s="10">
+      <c r="B243" s="9">
         <v>1412117305.3</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A244" s="11">
+      <c r="A244" s="10">
         <v>43709</v>
       </c>
-      <c r="B244" s="10">
+      <c r="B244" s="9">
         <v>1402192857.8199999</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A245" s="11">
+      <c r="A245" s="10">
         <v>43739</v>
       </c>
-      <c r="B245" s="10">
+      <c r="B245" s="9">
         <v>1401508788.95</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A246" s="11">
+      <c r="A246" s="10">
         <v>43770</v>
       </c>
-      <c r="B246" s="10">
+      <c r="B246" s="9">
         <v>1442560805.0599999</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A247" s="11">
+      <c r="A247" s="10">
         <v>43800</v>
       </c>
-      <c r="B247" s="10">
+      <c r="B247" s="9">
         <v>1548852405.04</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A248" s="11">
+      <c r="A248" s="10">
         <v>43831</v>
       </c>
-      <c r="B248" s="10">
+      <c r="B248" s="9">
         <v>1527157236.6199999</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A249" s="11">
+      <c r="A249" s="10">
         <v>43862</v>
       </c>
-      <c r="B249" s="10">
+      <c r="B249" s="9">
         <v>1513835901.4400001</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A250" s="11">
+      <c r="A250" s="10">
         <v>43891</v>
       </c>
-      <c r="B250" s="10">
+      <c r="B250" s="9">
         <v>1565801350.78</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A251" s="11">
+      <c r="A251" s="10">
         <v>43922</v>
       </c>
-      <c r="B251" s="10">
+      <c r="B251" s="9">
         <v>1625892008.5999999</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A252" s="11">
+      <c r="A252" s="10">
         <v>43952</v>
       </c>
-      <c r="B252" s="10">
+      <c r="B252" s="9">
         <v>1682585669.9200001</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A253" s="11">
+      <c r="A253" s="10">
         <v>43983</v>
       </c>
-      <c r="B253" s="10">
+      <c r="B253" s="9">
         <v>1702400180.99</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A254" s="11">
+      <c r="A254" s="10">
         <v>44013</v>
       </c>
-      <c r="B254" s="10">
+      <c r="B254" s="9">
         <v>1750245495.96</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A255" s="11">
+      <c r="A255" s="10">
         <v>44044</v>
       </c>
-      <c r="B255" s="10">
+      <c r="B255" s="9">
         <v>1748034523.77</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A256" s="11">
+      <c r="A256" s="10">
         <v>44075</v>
       </c>
-      <c r="B256" s="10">
+      <c r="B256" s="9">
         <v>1729505390.8499999</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A257" s="11">
+      <c r="A257" s="10">
         <v>44105</v>
       </c>
-      <c r="B257" s="10">
+      <c r="B257" s="9">
         <v>1752524750.75</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A258" s="11">
+      <c r="A258" s="10">
         <v>44136</v>
       </c>
-      <c r="B258" s="10">
+      <c r="B258" s="9">
         <v>1784543870.02</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A259" s="11">
+      <c r="A259" s="10">
         <v>44166</v>
       </c>
-      <c r="B259" s="10">
+      <c r="B259" s="9">
         <v>1905669553.3</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A260" s="11">
+      <c r="A260" s="10">
         <v>44197</v>
       </c>
-      <c r="B260" s="10">
+      <c r="B260" s="9">
         <v>1901282565.72</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A261" s="11">
+      <c r="A261" s="10">
         <v>44228</v>
       </c>
-      <c r="B261" s="10">
+      <c r="B261" s="9">
         <v>1899154046.0799999</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A262" s="11">
+      <c r="A262" s="10">
         <v>44256</v>
       </c>
-      <c r="B262" s="10">
+      <c r="B262" s="9">
         <v>1963052006.1300001</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A263" s="11">
+      <c r="A263" s="10">
         <v>44287</v>
       </c>
-      <c r="B263" s="10">
+      <c r="B263" s="9">
         <v>1952963384.8299999</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A264" s="11">
+      <c r="A264" s="10">
         <v>44317</v>
       </c>
-      <c r="B264" s="10">
+      <c r="B264" s="9">
         <v>1966908774.3499999</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A265" s="11">
+      <c r="A265" s="10">
         <v>44348</v>
       </c>
-      <c r="B265" s="10">
+      <c r="B265" s="9">
         <v>1967008915.25</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A266" s="11">
+      <c r="A266" s="10">
         <v>44378</v>
       </c>
-      <c r="B266" s="10">
+      <c r="B266" s="9">
         <v>1992064200.9400001</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A267" s="11">
+      <c r="A267" s="10">
         <v>44409</v>
       </c>
-      <c r="B267" s="10">
+      <c r="B267" s="9">
         <v>1990292199.8699999</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A268" s="11">
+      <c r="A268" s="10">
         <v>44440</v>
       </c>
-      <c r="B268" s="10">
+      <c r="B268" s="9">
         <v>2005680537.9100001</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A269" s="11">
+      <c r="A269" s="10">
         <v>44470</v>
       </c>
-      <c r="B269" s="10">
+      <c r="B269" s="9">
         <v>2035818565.8699999</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A270" s="11">
+      <c r="A270" s="10">
         <v>44501</v>
       </c>
-      <c r="B270" s="10">
+      <c r="B270" s="9">
         <v>2082267855.4100001</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A271" s="11">
+      <c r="A271" s="10">
         <v>44531</v>
       </c>
-      <c r="B271" s="10">
+      <c r="B271" s="9">
         <v>2226643955.6199999</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A272" s="11">
+      <c r="A272" s="10">
         <v>44562</v>
       </c>
-      <c r="B272" s="10">
+      <c r="B272" s="9">
         <v>2225834477.8800001</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A273" s="11">
+      <c r="A273" s="10">
         <v>44593</v>
       </c>
-      <c r="B273" s="10">
+      <c r="B273" s="9">
         <v>2232413278.9400001</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A274" s="11">
+      <c r="A274" s="10">
         <v>44621</v>
       </c>
-      <c r="B274" s="10">
+      <c r="B274" s="9">
         <v>2265925780.2399998</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" s="11">
+      <c r="A275" s="10">
         <v>44652</v>
       </c>
-      <c r="B275" s="10">
+      <c r="B275" s="9">
         <v>2262570282.7399998</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A276" s="11">
+      <c r="A276" s="10">
         <v>44682</v>
       </c>
-      <c r="B276" s="10">
-        <v>2264556344.3099999</v>
+      <c r="B276" s="9">
+        <v>2264554650.3800001</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" s="11">
+      <c r="A277" s="10">
         <v>44713</v>
       </c>
-      <c r="B277" s="10">
-        <v>2257605809.3099999</v>
-      </c>
+      <c r="B277" s="9">
+        <v>2257660864.02</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" s="10">
+        <v>44743</v>
+      </c>
+      <c r="B278" s="9">
+        <v>2297308886.9000001</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="10">
+        <v>44774</v>
+      </c>
+      <c r="B279" s="9">
+        <v>2270113845.21</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="10">
+        <v>44805</v>
+      </c>
+      <c r="B280" s="9">
+        <v>2289233953.6199999</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="10">
+        <v>44835</v>
+      </c>
+      <c r="B281" s="9">
+        <v>2297638222.0100002</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="10">
+        <v>44866</v>
+      </c>
+      <c r="B282" s="9">
+        <v>2331301320.46</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" s="10">
+        <v>44896</v>
+      </c>
+      <c r="B283" s="9">
+        <v>2474683442.46</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="11"/>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" s="11"/>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286" s="11"/>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" s="11"/>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288" s="11"/>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" s="11"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" s="11"/>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291" s="11"/>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292" s="11"/>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293" s="11"/>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294" s="11"/>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295" s="11"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296" s="11"/>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297" s="11"/>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298" s="11"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299" s="11"/>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" s="11"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301" s="11"/>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302" s="11"/>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A303" s="11"/>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A304" s="11"/>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A305" s="11"/>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A306" s="11"/>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A307" s="11"/>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A308" s="11"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A309" s="11"/>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A310" s="11"/>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A311" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>